<commit_message>
Update edited session - 2025-09-29T08:28:53.865Z - Cache Bust ID: 1759134533865h5h496kdg
</commit_message>
<xml_diff>
--- a/log_history/Y2_B2526_Pharmacology_scanner1759131721293_c34025bd37256db81f2c1a1cb53ba3c52790919084614c0186f370c76671ad4a.xlsx
+++ b/log_history/Y2_B2526_Pharmacology_scanner1759131721293_c34025bd37256db81f2c1a1cb53ba3c52790919084614c0186f370c76671ad4a.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -964,7 +964,7 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>234537</v>
+        <v>234699</v>
       </c>
       <c r="B29" t="str">
         <v>Pharmacology</v>
@@ -973,7 +973,7 @@
         <v>29/09/2025</v>
       </c>
       <c r="D29" t="str">
-        <v>11:04:06</v>
+        <v>11:04:11</v>
       </c>
       <c r="E29" t="str">
         <v>Manual</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>234699</v>
+        <v>234810</v>
       </c>
       <c r="B30" t="str">
         <v>Pharmacology</v>
@@ -993,7 +993,7 @@
         <v>29/09/2025</v>
       </c>
       <c r="D30" t="str">
-        <v>11:04:11</v>
+        <v>11:09:30</v>
       </c>
       <c r="E30" t="str">
         <v>Manual</v>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>234810</v>
+        <v>234687</v>
       </c>
       <c r="B31" t="str">
         <v>Pharmacology</v>
@@ -1013,7 +1013,7 @@
         <v>29/09/2025</v>
       </c>
       <c r="D31" t="str">
-        <v>11:09:30</v>
+        <v>11:09:40</v>
       </c>
       <c r="E31" t="str">
         <v>Manual</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>234687</v>
+        <v>234683</v>
       </c>
       <c r="B32" t="str">
         <v>Pharmacology</v>
@@ -1033,7 +1033,7 @@
         <v>29/09/2025</v>
       </c>
       <c r="D32" t="str">
-        <v>11:09:40</v>
+        <v>11:09:43</v>
       </c>
       <c r="E32" t="str">
         <v>Manual</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>234683</v>
+        <v>234816</v>
       </c>
       <c r="B33" t="str">
         <v>Pharmacology</v>
@@ -1053,7 +1053,7 @@
         <v>29/09/2025</v>
       </c>
       <c r="D33" t="str">
-        <v>11:09:43</v>
+        <v>11:09:55</v>
       </c>
       <c r="E33" t="str">
         <v>Manual</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>234816</v>
+        <v>234651</v>
       </c>
       <c r="B34" t="str">
         <v>Pharmacology</v>
@@ -1073,7 +1073,7 @@
         <v>29/09/2025</v>
       </c>
       <c r="D34" t="str">
-        <v>11:09:55</v>
+        <v>11:10:00</v>
       </c>
       <c r="E34" t="str">
         <v>Manual</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>234651</v>
+        <v>234452</v>
       </c>
       <c r="B35" t="str">
         <v>Pharmacology</v>
@@ -1093,7 +1093,7 @@
         <v>29/09/2025</v>
       </c>
       <c r="D35" t="str">
-        <v>11:10:00</v>
+        <v>11:10:06</v>
       </c>
       <c r="E35" t="str">
         <v>Manual</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>234452</v>
+        <v>234702</v>
       </c>
       <c r="B36" t="str">
         <v>Pharmacology</v>
@@ -1113,7 +1113,7 @@
         <v>29/09/2025</v>
       </c>
       <c r="D36" t="str">
-        <v>11:10:06</v>
+        <v>11:10:21</v>
       </c>
       <c r="E36" t="str">
         <v>Manual</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>234702</v>
+        <v>234387</v>
       </c>
       <c r="B37" t="str">
         <v>Pharmacology</v>
@@ -1133,7 +1133,7 @@
         <v>29/09/2025</v>
       </c>
       <c r="D37" t="str">
-        <v>11:10:21</v>
+        <v>11:10:26</v>
       </c>
       <c r="E37" t="str">
         <v>Manual</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>234387</v>
+        <v>235148</v>
       </c>
       <c r="B38" t="str">
         <v>Pharmacology</v>
@@ -1153,7 +1153,7 @@
         <v>29/09/2025</v>
       </c>
       <c r="D38" t="str">
-        <v>11:10:26</v>
+        <v>11:10:36</v>
       </c>
       <c r="E38" t="str">
         <v>Manual</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>235148</v>
+        <v>234267</v>
       </c>
       <c r="B39" t="str">
         <v>Pharmacology</v>
@@ -1173,7 +1173,7 @@
         <v>29/09/2025</v>
       </c>
       <c r="D39" t="str">
-        <v>11:10:36</v>
+        <v>11:10:50</v>
       </c>
       <c r="E39" t="str">
         <v>Manual</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>234267</v>
+        <v>234273</v>
       </c>
       <c r="B40" t="str">
         <v>Pharmacology</v>
@@ -1193,7 +1193,7 @@
         <v>29/09/2025</v>
       </c>
       <c r="D40" t="str">
-        <v>11:10:50</v>
+        <v>11:10:55</v>
       </c>
       <c r="E40" t="str">
         <v>Manual</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>234273</v>
+        <v>235105</v>
       </c>
       <c r="B41" t="str">
         <v>Pharmacology</v>
@@ -1213,7 +1213,7 @@
         <v>29/09/2025</v>
       </c>
       <c r="D41" t="str">
-        <v>11:10:55</v>
+        <v>11:11:13</v>
       </c>
       <c r="E41" t="str">
         <v>Manual</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>235105</v>
+        <v>235103</v>
       </c>
       <c r="B42" t="str">
         <v>Pharmacology</v>
@@ -1233,7 +1233,7 @@
         <v>29/09/2025</v>
       </c>
       <c r="D42" t="str">
-        <v>11:11:13</v>
+        <v>11:11:21</v>
       </c>
       <c r="E42" t="str">
         <v>Manual</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>235103</v>
+        <v>234678</v>
       </c>
       <c r="B43" t="str">
         <v>Pharmacology</v>
@@ -1253,7 +1253,7 @@
         <v>29/09/2025</v>
       </c>
       <c r="D43" t="str">
-        <v>11:11:21</v>
+        <v>11:11:31</v>
       </c>
       <c r="E43" t="str">
         <v>Manual</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>234678</v>
+        <v>234843</v>
       </c>
       <c r="B44" t="str">
         <v>Pharmacology</v>
@@ -1273,7 +1273,7 @@
         <v>29/09/2025</v>
       </c>
       <c r="D44" t="str">
-        <v>11:11:31</v>
+        <v>11:11:42</v>
       </c>
       <c r="E44" t="str">
         <v>Manual</v>
@@ -1284,7 +1284,7 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>234843</v>
+        <v>234698</v>
       </c>
       <c r="B45" t="str">
         <v>Pharmacology</v>
@@ -1293,38 +1293,18 @@
         <v>29/09/2025</v>
       </c>
       <c r="D45" t="str">
-        <v>11:11:42</v>
+        <v>11:12:34</v>
       </c>
       <c r="E45" t="str">
         <v>Manual</v>
       </c>
       <c r="F45" t="str">
-        <v>nourhan.mostafa@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="str">
-        <v>234698</v>
-      </c>
-      <c r="B46" t="str">
-        <v>Pharmacology</v>
-      </c>
-      <c r="C46" t="str">
-        <v>29/09/2025</v>
-      </c>
-      <c r="D46" t="str">
-        <v>11:12:34</v>
-      </c>
-      <c r="E46" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F46" t="str">
         <v>nourhan.mostafa@med.asu.edu.eg</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F46"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F45"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>